<commit_message>
done with hw 7 part 1
</commit_message>
<xml_diff>
--- a/Feb. 24 In-Class Problems.xlsx
+++ b/Feb. 24 In-Class Problems.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example 6-5" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Example 6-7" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve">MARR = </t>
   </si>
@@ -132,6 +133,27 @@
   <si>
     <t xml:space="preserve">Solution using incremental analysis using RATE and PV Functions</t>
   </si>
+  <si>
+    <t xml:space="preserve">MARR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital Investmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual Cash Flows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useful Life (Years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market Value</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +171,7 @@
     <numFmt numFmtId="172" formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="173" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -214,7 +236,12 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Times New Roman"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -275,7 +302,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -304,10 +331,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,10 +391,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,6 +400,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,9 +498,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>532800</xdr:colOff>
+      <xdr:colOff>532080</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -478,8 +509,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7824240" y="152280"/>
-          <a:ext cx="8886600" cy="3412440"/>
+          <a:off x="7818120" y="152280"/>
+          <a:ext cx="8886600" cy="3407400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -591,9 +622,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>806760</xdr:colOff>
+      <xdr:colOff>806040</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -606,8 +637,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7829280" y="3835800"/>
-          <a:ext cx="6970320" cy="2378880"/>
+          <a:off x="7823160" y="3835800"/>
+          <a:ext cx="6969240" cy="2378160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -629,13 +660,13 @@
   </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="17.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="17.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="21.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="20.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="1" width="12.73"/>
@@ -658,12 +689,12 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,42 +705,42 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" s="12" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9" t="s">
+    <row r="4" s="11" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="34.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="12" t="n">
         <v>-100000</v>
       </c>
-      <c r="C5" s="13" t="n">
+      <c r="C5" s="12" t="n">
         <v>-140600</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="12" t="n">
         <v>-148200</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E5" s="12" t="n">
         <v>-122000</v>
       </c>
       <c r="F5" s="3"/>
@@ -718,16 +749,16 @@
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13" t="n">
+      <c r="B6" s="12" t="n">
         <v>-29000</v>
       </c>
-      <c r="C6" s="13" t="n">
+      <c r="C6" s="12" t="n">
         <v>-16900</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D6" s="12" t="n">
         <v>-14800</v>
       </c>
-      <c r="E6" s="13" t="n">
+      <c r="E6" s="12" t="n">
         <v>-22100</v>
       </c>
       <c r="F6" s="3"/>
@@ -736,186 +767,186 @@
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14" t="n">
+      <c r="B7" s="13" t="n">
         <v>10000</v>
       </c>
-      <c r="C7" s="14" t="n">
+      <c r="C7" s="13" t="n">
         <v>14000</v>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="13" t="n">
         <v>25600</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="13" t="n">
         <v>14000</v>
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" s="12" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+    <row r="8" s="11" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E8" s="9" t="n">
+      <c r="E8" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="B11" s="13" t="n">
+      <c r="B11" s="12" t="n">
         <f aca="false">E5 - B5</f>
         <v>-22000</v>
       </c>
-      <c r="C11" s="13" t="n">
+      <c r="C11" s="12" t="n">
         <f aca="false">C5-E5</f>
         <v>-18600</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="12" t="n">
         <f aca="false">D5-E5</f>
         <v>-26200</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="13" t="n">
+      <c r="B12" s="12" t="n">
         <f aca="false">E$6 - B$6</f>
         <v>6900</v>
       </c>
-      <c r="C12" s="13" t="n">
+      <c r="C12" s="12" t="n">
         <f aca="false">$C$6-$E$6</f>
         <v>5200</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D12" s="12" t="n">
         <f aca="false">$D$6-$E$6</f>
         <v>7300</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B13" s="13" t="n">
+      <c r="B13" s="12" t="n">
         <f aca="false">E$6 - B$6</f>
         <v>6900</v>
       </c>
-      <c r="C13" s="13" t="n">
+      <c r="C13" s="12" t="n">
         <f aca="false">$C$6-$E$6</f>
         <v>5200</v>
       </c>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="12" t="n">
         <f aca="false">$D$6-$E$6</f>
         <v>7300</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B14" s="13" t="n">
+      <c r="B14" s="12" t="n">
         <f aca="false">E$6 - B$6</f>
         <v>6900</v>
       </c>
-      <c r="C14" s="13" t="n">
+      <c r="C14" s="12" t="n">
         <f aca="false">$C$6-$E$6</f>
         <v>5200</v>
       </c>
-      <c r="D14" s="13" t="n">
+      <c r="D14" s="12" t="n">
         <f aca="false">$D$6-$E$6</f>
         <v>7300</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B15" s="13" t="n">
+      <c r="B15" s="12" t="n">
         <f aca="false">E$6 - B$6</f>
         <v>6900</v>
       </c>
-      <c r="C15" s="13" t="n">
+      <c r="C15" s="12" t="n">
         <f aca="false">$C$6-$E$6</f>
         <v>5200</v>
       </c>
-      <c r="D15" s="13" t="n">
+      <c r="D15" s="12" t="n">
         <f aca="false">$D$6-$E$6</f>
         <v>7300</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B16" s="13" t="n">
+      <c r="B16" s="12" t="n">
         <f aca="false">E$6 - B$6 + (E7 - B7)</f>
         <v>10900</v>
       </c>
-      <c r="C16" s="13" t="n">
+      <c r="C16" s="12" t="n">
         <f aca="false">$C$6-$E$6+(C7-E7)</f>
         <v>5200</v>
       </c>
-      <c r="D16" s="13" t="n">
+      <c r="D16" s="12" t="n">
         <f aca="false">$D$6-$E$6 + (D7-E7)</f>
         <v>18900</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -923,108 +954,108 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="19" t="n">
+      <c r="B18" s="18" t="n">
         <f aca="false">IRR(B11:B16)</f>
         <v>0.204700431840086</v>
       </c>
-      <c r="C18" s="19" t="n">
+      <c r="C18" s="18" t="n">
         <f aca="false">IRR(C11:C16)</f>
         <v>0.123138600909013</v>
       </c>
-      <c r="D18" s="19" t="n">
+      <c r="D18" s="18" t="n">
         <f aca="false">IRR(D11:D16)</f>
         <v>0.204385298032041</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="20" t="n">
+      <c r="B19" s="19" t="n">
         <f aca="false">NPV($B$1, B12:B16)+B11</f>
         <v>242.734053497945</v>
       </c>
-      <c r="C19" s="20" t="n">
+      <c r="C19" s="19" t="n">
         <f aca="false">NPV($B$1, C12:C16)+C11</f>
         <v>-3048.81687242798</v>
       </c>
-      <c r="D19" s="20" t="n">
+      <c r="D19" s="19" t="n">
         <f aca="false">NPV($B$1, D12:D16)+D11</f>
         <v>293.248456790127</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="19" t="n">
+      <c r="B24" s="18" t="n">
         <f aca="false">RATE($B$2,(E6-B6), (E5-B5),(E7-B7))</f>
         <v>0.204700431840086</v>
       </c>
-      <c r="C24" s="19" t="n">
+      <c r="C24" s="18" t="n">
         <f aca="false">RATE($B$2,(C6-E6),(C5-E5),(C7-E7))</f>
         <v>0.123138600909013</v>
       </c>
-      <c r="D24" s="19" t="n">
+      <c r="D24" s="18" t="n">
         <f aca="false">RATE(B2,(D6-E6),(D5-E5),(D7-E7))</f>
         <v>0.204385298032041</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="20" t="n">
+      <c r="B25" s="19" t="n">
         <f aca="false">PV(B1,B2,-(E6-B6),-(E7-B7)) + (E5-B5)</f>
         <v>242.734053497941</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="19" t="n">
         <f aca="false">PV(B1,B2,-(C6-E6),-(C7-E7)) + (C5-E5)</f>
         <v>-3048.81687242798</v>
       </c>
-      <c r="D25" s="25" t="n">
+      <c r="D25" s="23" t="n">
         <f aca="false">PV(B1,B2,-(D6-E6),-(D7-E7)) + (D5-E5)</f>
         <v>293.248456790119</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G26" s="26"/>
+      <c r="G26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1040,4 +1071,90 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="26" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="27" t="n">
+        <f aca="false">-3500</f>
+        <v>-3500</v>
+      </c>
+      <c r="D4" s="27" t="n">
+        <f aca="false">-5000</f>
+        <v>-5000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="27" t="n">
+        <v>1255</v>
+      </c>
+      <c r="D5" s="27" t="n">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="25" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>